<commit_message>
Add unittest for holten-cityjet wr.ar3
</commit_message>
<xml_diff>
--- a/Route66/Documents/FOS lijst AutoLogic 2017 2018.xlsx
+++ b/Route66/Documents/FOS lijst AutoLogic 2017 2018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="309">
   <si>
     <t>Nr.</t>
   </si>
@@ -1079,9 +1079,6 @@
     <t xml:space="preserve"> Voorbeeld route G1-P-10_H_ASH23012017.ALR in RouteCreator wordt geen startpunt getoond in de tabel NP. Wel op kaart.</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>opmerking</t>
   </si>
   <si>
@@ -1148,10 +1145,37 @@
     <t>Niet nodig in route66</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>GPS marker kunnen via menu aan/uit gezet worden.</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>navteq wordt niet meer gebruikt</t>
+  </si>
+  <si>
+    <t>Knippen /plakken gaat nu via Ctrl-X, Ctrl-V</t>
+  </si>
+  <si>
+    <t>Kaart wordt automatisch gecentreerd bij openen bestand.</t>
+  </si>
+  <si>
+    <t>markers worden m.b.v. Del toets verwijderd.</t>
+  </si>
+  <si>
+    <t>Kaarten worden automatisch van server gehaald.</t>
+  </si>
+  <si>
+    <t>Er verschijnt een status melding (in rood) wanneer route geen GPS markers bevat.</t>
+  </si>
+  <si>
+    <t>AR0 laten vervallen?  Kan wat betreft route66.</t>
+  </si>
+  <si>
+    <t>Via Ctrl-O kun je pad opgeven. Laatste gebruikte pad wordt onthouden.</t>
   </si>
 </sst>
 </file>
@@ -1409,30 +1433,6 @@
   <dxfs count="18">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1525,6 +1525,30 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2139,9 +2163,9 @@
         <filter val="RouteCreator"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="2">
+    <filterColumn colId="9">
       <filters>
-        <filter val="Wens"/>
+        <filter val="Open"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2159,12 +2183,12 @@
     <tableColumn id="6" name="Datum" dataDxfId="8"/>
     <tableColumn id="11" name="Prio" dataDxfId="7"/>
     <tableColumn id="15" name="Route66" dataDxfId="6"/>
-    <tableColumn id="16" name="opmerking" dataDxfId="0"/>
-    <tableColumn id="7" name="Status" dataDxfId="5"/>
-    <tableColumn id="14" name="Datum afgehandeld" dataDxfId="4"/>
-    <tableColumn id="8" name="Afbeelding" dataDxfId="3"/>
-    <tableColumn id="9" name="Jira Item / geescaleerd?" dataDxfId="2"/>
-    <tableColumn id="13" name="Extra toelichting" dataDxfId="1"/>
+    <tableColumn id="16" name="opmerking" dataDxfId="5"/>
+    <tableColumn id="7" name="Status" dataDxfId="4"/>
+    <tableColumn id="14" name="Datum afgehandeld" dataDxfId="3"/>
+    <tableColumn id="8" name="Afbeelding" dataDxfId="2"/>
+    <tableColumn id="9" name="Jira Item / geescaleerd?" dataDxfId="1"/>
+    <tableColumn id="13" name="Extra toelichting" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2466,7 +2490,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J86" sqref="J86"/>
+      <selection pane="bottomRight" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -2479,11 +2503,11 @@
     <col min="6" max="6" width="9.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.109375" style="22" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="5" style="22" customWidth="1"/>
-    <col min="10" max="10" width="11" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" style="27" customWidth="1"/>
-    <col min="12" max="12" width="39.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" style="22" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="31.88671875" style="27" customWidth="1"/>
+    <col min="12" max="12" width="39.109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="12" style="5" customWidth="1"/>
     <col min="15" max="15" width="23.6640625" style="25" customWidth="1"/>
     <col min="16" max="16" width="83.5546875" style="5" customWidth="1"/>
@@ -2521,7 +2545,7 @@
         <v>273</v>
       </c>
       <c r="K1" s="55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>5</v>
@@ -2568,7 +2592,9 @@
       <c r="J2" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="18" t="s">
+        <v>306</v>
+      </c>
       <c r="L2" s="15" t="s">
         <v>218</v>
       </c>
@@ -2577,7 +2603,7 @@
       <c r="O2" s="18"/>
       <c r="P2" s="15"/>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A3" s="26">
         <v>4</v>
       </c>
@@ -2607,7 +2633,7 @@
         <v>274</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>193</v>
@@ -2695,7 +2721,7 @@
       </c>
       <c r="P5" s="15"/>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A6" s="26">
         <v>9</v>
       </c>
@@ -2725,7 +2751,7 @@
         <v>274</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>188</v>
@@ -2766,7 +2792,9 @@
       <c r="J7" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K7" s="15"/>
+      <c r="K7" s="18" t="s">
+        <v>305</v>
+      </c>
       <c r="L7" s="15" t="s">
         <v>193</v>
       </c>
@@ -2842,7 +2870,9 @@
       <c r="J9" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="18" t="s">
+        <v>302</v>
+      </c>
       <c r="L9" s="15" t="s">
         <v>188</v>
       </c>
@@ -2853,7 +2883,7 @@
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
     </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="10" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A10" s="26">
         <v>17</v>
       </c>
@@ -2883,7 +2913,7 @@
         <v>274</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>188</v>
@@ -2926,7 +2956,9 @@
       <c r="J11" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="L11" s="15" t="s">
         <v>188</v>
       </c>
@@ -3074,7 +3106,9 @@
       <c r="J15" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="18" t="s">
+        <v>304</v>
+      </c>
       <c r="L15" s="15" t="s">
         <v>218</v>
       </c>
@@ -3155,7 +3189,7 @@
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
     </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A18" s="26">
         <v>35</v>
       </c>
@@ -3182,10 +3216,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L18" s="15" t="s">
         <v>193</v>
@@ -3195,7 +3229,7 @@
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
     </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A19" s="26">
         <v>36</v>
       </c>
@@ -3225,7 +3259,7 @@
         <v>274</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>188</v>
@@ -3237,7 +3271,7 @@
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:16" s="2" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A20" s="26">
         <v>38</v>
       </c>
@@ -3267,7 +3301,7 @@
         <v>274</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L20" s="15" t="s">
         <v>193</v>
@@ -3414,7 +3448,7 @@
       <c r="J24" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K24" s="15"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="15" t="s">
         <v>188</v>
       </c>
@@ -3456,7 +3490,7 @@
       <c r="J25" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K25" s="15"/>
+      <c r="K25" s="18"/>
       <c r="L25" s="15" t="s">
         <v>218</v>
       </c>
@@ -3494,7 +3528,7 @@
       <c r="J26" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K26" s="15"/>
+      <c r="K26" s="18"/>
       <c r="L26" s="15" t="s">
         <v>218</v>
       </c>
@@ -3532,7 +3566,7 @@
       <c r="J27" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K27" s="15"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="15" t="s">
         <v>193</v>
       </c>
@@ -3653,7 +3687,7 @@
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="31" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A31" s="26">
         <v>76</v>
       </c>
@@ -3679,8 +3713,10 @@
       <c r="I31" s="15">
         <v>1</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+      <c r="J31" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="K31" s="18"/>
       <c r="L31" s="15" t="s">
         <v>218</v>
       </c>
@@ -3720,7 +3756,7 @@
       <c r="J32" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K32" s="15"/>
+      <c r="K32" s="18"/>
       <c r="L32" s="15" t="s">
         <v>218</v>
       </c>
@@ -3760,7 +3796,7 @@
       <c r="J33" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K33" s="15"/>
+      <c r="K33" s="18"/>
       <c r="L33" s="15" t="s">
         <v>188</v>
       </c>
@@ -3800,7 +3836,7 @@
       <c r="J34" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K34" s="15"/>
+      <c r="K34" s="18"/>
       <c r="L34" s="15" t="s">
         <v>218</v>
       </c>
@@ -3809,7 +3845,7 @@
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
     </row>
-    <row r="35" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="35" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A35" s="26">
         <v>97</v>
       </c>
@@ -3839,7 +3875,7 @@
         <v>274</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L35" s="15" t="s">
         <v>188</v>
@@ -3851,7 +3887,7 @@
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
     </row>
-    <row r="36" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="36" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A36" s="26">
         <v>98</v>
       </c>
@@ -3881,7 +3917,7 @@
         <v>274</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L36" s="15" t="s">
         <v>193</v>
@@ -3891,7 +3927,7 @@
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
     </row>
-    <row r="37" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="37" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A37" s="26">
         <v>99</v>
       </c>
@@ -3921,7 +3957,7 @@
         <v>274</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L37" s="15" t="s">
         <v>193</v>
@@ -3931,7 +3967,7 @@
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
     </row>
-    <row r="38" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="38" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A38" s="26">
         <v>100</v>
       </c>
@@ -3961,7 +3997,7 @@
         <v>274</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L38" s="15" t="s">
         <v>193</v>
@@ -3971,7 +4007,7 @@
       <c r="O38" s="15"/>
       <c r="P38" s="15"/>
     </row>
-    <row r="39" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="39" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A39" s="26">
         <v>101</v>
       </c>
@@ -4001,7 +4037,7 @@
         <v>274</v>
       </c>
       <c r="K39" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L39" s="15" t="s">
         <v>193</v>
@@ -4011,7 +4047,7 @@
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
     </row>
-    <row r="40" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="40" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A40" s="26">
         <v>103</v>
       </c>
@@ -4041,7 +4077,7 @@
         <v>274</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>188</v>
@@ -4091,7 +4127,7 @@
       <c r="O41" s="15"/>
       <c r="P41" s="15"/>
     </row>
-    <row r="42" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="42" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A42" s="26">
         <v>104</v>
       </c>
@@ -4121,7 +4157,7 @@
         <v>274</v>
       </c>
       <c r="K42" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L42" s="15" t="s">
         <v>188</v>
@@ -4133,7 +4169,7 @@
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
     </row>
-    <row r="43" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="43" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A43" s="26">
         <v>105</v>
       </c>
@@ -4163,7 +4199,7 @@
         <v>274</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L43" s="15" t="s">
         <v>188</v>
@@ -4175,7 +4211,7 @@
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
     </row>
-    <row r="44" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="44" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A44" s="26">
         <v>106</v>
       </c>
@@ -4205,7 +4241,7 @@
         <v>274</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L44" s="15" t="s">
         <v>218</v>
@@ -4395,7 +4431,7 @@
       <c r="O49" s="15"/>
       <c r="P49" s="15"/>
     </row>
-    <row r="50" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="50" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A50" s="26">
         <v>107</v>
       </c>
@@ -4425,7 +4461,7 @@
         <v>274</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L50" s="15" t="s">
         <v>218</v>
@@ -4435,7 +4471,7 @@
       <c r="O50" s="15"/>
       <c r="P50" s="15"/>
     </row>
-    <row r="51" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="51" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A51" s="26">
         <v>108</v>
       </c>
@@ -4465,7 +4501,7 @@
         <v>274</v>
       </c>
       <c r="K51" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L51" s="15" t="s">
         <v>218</v>
@@ -4504,7 +4540,7 @@
       <c r="J52" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K52" s="20"/>
+      <c r="K52" s="30"/>
       <c r="L52" s="20" t="s">
         <v>193</v>
       </c>
@@ -4578,7 +4614,7 @@
       <c r="J54" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K54" s="20"/>
+      <c r="K54" s="30"/>
       <c r="L54" s="20" t="s">
         <v>193</v>
       </c>
@@ -4618,7 +4654,7 @@
       <c r="J55" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K55" s="15"/>
+      <c r="K55" s="18"/>
       <c r="L55" s="15" t="s">
         <v>188</v>
       </c>
@@ -4701,7 +4737,7 @@
       <c r="O57" s="15"/>
       <c r="P57" s="15"/>
     </row>
-    <row r="58" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="58" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A58" s="45">
         <v>119</v>
       </c>
@@ -4731,7 +4767,7 @@
         <v>274</v>
       </c>
       <c r="K58" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L58" s="46" t="s">
         <v>193</v>
@@ -4808,7 +4844,7 @@
       <c r="J60" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K60" s="15"/>
+      <c r="K60" s="18"/>
       <c r="L60" s="6" t="s">
         <v>188</v>
       </c>
@@ -4886,7 +4922,7 @@
       <c r="J62" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K62" s="20"/>
+      <c r="K62" s="30"/>
       <c r="L62" s="46" t="s">
         <v>188</v>
       </c>
@@ -4959,8 +4995,10 @@
       <c r="I64" s="15">
         <v>1</v>
       </c>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
+      <c r="J64" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="K64" s="18"/>
       <c r="L64" s="6" t="s">
         <v>268</v>
       </c>
@@ -4999,7 +5037,7 @@
         <v>193</v>
       </c>
       <c r="K65" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L65" s="15" t="s">
         <v>193</v>
@@ -5362,7 +5400,7 @@
       <c r="J75" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K75" s="15"/>
+      <c r="K75" s="18"/>
       <c r="L75" s="15" t="s">
         <v>188</v>
       </c>
@@ -5404,7 +5442,7 @@
       <c r="J76" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K76" s="15"/>
+      <c r="K76" s="18"/>
       <c r="L76" s="15" t="s">
         <v>193</v>
       </c>
@@ -5413,7 +5451,7 @@
       <c r="O76" s="15"/>
       <c r="P76" s="15"/>
     </row>
-    <row r="77" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="77" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A77" s="26">
         <v>19</v>
       </c>
@@ -5453,7 +5491,7 @@
       <c r="O77" s="15"/>
       <c r="P77" s="15"/>
     </row>
-    <row r="78" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="78" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A78" s="26">
         <v>23</v>
       </c>
@@ -5481,7 +5519,7 @@
         <v>274</v>
       </c>
       <c r="K78" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L78" s="15" t="s">
         <v>193</v>
@@ -5527,7 +5565,7 @@
       <c r="O79" s="15"/>
       <c r="P79" s="15"/>
     </row>
-    <row r="80" spans="1:16" s="3" customFormat="1" ht="92.25" customHeight="1">
+    <row r="80" spans="1:16" s="3" customFormat="1" ht="92.25" hidden="1" customHeight="1">
       <c r="A80" s="26">
         <v>26</v>
       </c>
@@ -5603,7 +5641,7 @@
       <c r="O81" s="15"/>
       <c r="P81" s="15"/>
     </row>
-    <row r="82" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="82" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A82" s="26">
         <v>31</v>
       </c>
@@ -5633,7 +5671,7 @@
         <v>274</v>
       </c>
       <c r="K82" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L82" s="15" t="s">
         <v>193</v>
@@ -5672,7 +5710,7 @@
       <c r="J83" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K83" s="15"/>
+      <c r="K83" s="18"/>
       <c r="L83" s="15" t="s">
         <v>193</v>
       </c>
@@ -5710,7 +5748,7 @@
       <c r="J84" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K84" s="15"/>
+      <c r="K84" s="18"/>
       <c r="L84" s="15" t="s">
         <v>193</v>
       </c>
@@ -5750,7 +5788,7 @@
       <c r="J85" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K85" s="15"/>
+      <c r="K85" s="18"/>
       <c r="L85" s="15" t="s">
         <v>188</v>
       </c>
@@ -5763,7 +5801,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="86" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A86" s="26">
         <v>49</v>
       </c>
@@ -5789,7 +5827,9 @@
       <c r="I86" s="15">
         <v>2</v>
       </c>
-      <c r="J86" s="15"/>
+      <c r="J86" s="15" t="s">
+        <v>274</v>
+      </c>
       <c r="K86" s="18"/>
       <c r="L86" s="15" t="s">
         <v>193</v>
@@ -5799,7 +5839,7 @@
       <c r="O86" s="15"/>
       <c r="P86" s="15"/>
     </row>
-    <row r="87" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="87" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A87" s="26">
         <v>51</v>
       </c>
@@ -5826,9 +5866,11 @@
         <v>2</v>
       </c>
       <c r="J87" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="K87" s="15"/>
+        <v>193</v>
+      </c>
+      <c r="K87" s="18" t="s">
+        <v>307</v>
+      </c>
       <c r="L87" s="15" t="s">
         <v>193</v>
       </c>
@@ -5868,7 +5910,7 @@
       <c r="J88" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K88" s="15"/>
+      <c r="K88" s="18"/>
       <c r="L88" s="15" t="s">
         <v>193</v>
       </c>
@@ -5939,7 +5981,9 @@
       <c r="I90" s="15">
         <v>2</v>
       </c>
-      <c r="J90" s="15"/>
+      <c r="J90" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="K90" s="18"/>
       <c r="L90" s="15" t="s">
         <v>193</v>
@@ -6119,7 +6163,9 @@
       <c r="I95" s="15">
         <v>2</v>
       </c>
-      <c r="J95" s="15"/>
+      <c r="J95" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="K95" s="18"/>
       <c r="L95" s="15" t="s">
         <v>193</v>
@@ -6165,7 +6211,7 @@
       <c r="O96" s="15"/>
       <c r="P96" s="15"/>
     </row>
-    <row r="97" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="97" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A97" s="26">
         <v>63</v>
       </c>
@@ -6191,7 +6237,9 @@
       <c r="I97" s="15">
         <v>2</v>
       </c>
-      <c r="J97" s="15"/>
+      <c r="J97" s="15" t="s">
+        <v>274</v>
+      </c>
       <c r="K97" s="18"/>
       <c r="L97" s="15" t="s">
         <v>193</v>
@@ -6201,7 +6249,7 @@
       <c r="O97" s="15"/>
       <c r="P97" s="15"/>
     </row>
-    <row r="98" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="98" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A98" s="26">
         <v>79</v>
       </c>
@@ -6227,7 +6275,9 @@
       <c r="I98" s="15">
         <v>2</v>
       </c>
-      <c r="J98" s="15"/>
+      <c r="J98" s="15" t="s">
+        <v>300</v>
+      </c>
       <c r="K98" s="18"/>
       <c r="L98" s="15" t="s">
         <v>218</v>
@@ -6237,7 +6287,7 @@
       <c r="O98" s="15"/>
       <c r="P98" s="15"/>
     </row>
-    <row r="99" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="99" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A99" s="26">
         <v>81</v>
       </c>
@@ -6263,8 +6313,12 @@
       <c r="I99" s="15">
         <v>2</v>
       </c>
-      <c r="J99" s="15"/>
-      <c r="K99" s="18"/>
+      <c r="J99" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="K99" s="18" t="s">
+        <v>308</v>
+      </c>
       <c r="L99" s="15" t="s">
         <v>188</v>
       </c>
@@ -6304,7 +6358,7 @@
       <c r="J100" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K100" s="15"/>
+      <c r="K100" s="18"/>
       <c r="L100" s="15" t="s">
         <v>218</v>
       </c>
@@ -6313,7 +6367,7 @@
       <c r="O100" s="15"/>
       <c r="P100" s="15"/>
     </row>
-    <row r="101" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="101" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A101" s="26">
         <v>89</v>
       </c>
@@ -6351,7 +6405,7 @@
       <c r="O101" s="15"/>
       <c r="P101" s="15"/>
     </row>
-    <row r="102" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="102" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A102" s="26">
         <v>94</v>
       </c>
@@ -6418,7 +6472,7 @@
       <c r="J103" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K103" s="20"/>
+      <c r="K103" s="30"/>
       <c r="L103" s="20" t="s">
         <v>193</v>
       </c>
@@ -6494,7 +6548,7 @@
       <c r="J105" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K105" s="20"/>
+      <c r="K105" s="30"/>
       <c r="L105" s="20" t="s">
         <v>193</v>
       </c>
@@ -6570,7 +6624,7 @@
       <c r="J107" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="K107" s="20"/>
+      <c r="K107" s="30"/>
       <c r="L107" s="20" t="s">
         <v>193</v>
       </c>
@@ -6581,7 +6635,7 @@
       <c r="O107" s="20"/>
       <c r="P107" s="20"/>
     </row>
-    <row r="108" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="108" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A108" s="43">
         <v>122</v>
       </c>
@@ -6611,7 +6665,7 @@
         <v>274</v>
       </c>
       <c r="K108" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L108" s="6" t="s">
         <v>193</v>
@@ -6646,9 +6700,9 @@
         <v>2</v>
       </c>
       <c r="J109" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="K109" s="15"/>
+        <v>274</v>
+      </c>
+      <c r="K109" s="18"/>
       <c r="L109" s="6" t="s">
         <v>193</v>
       </c>
@@ -6717,7 +6771,9 @@
       <c r="I111" s="15">
         <v>3</v>
       </c>
-      <c r="J111" s="15"/>
+      <c r="J111" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="K111" s="18"/>
       <c r="L111" s="15" t="s">
         <v>193</v>
@@ -6727,7 +6783,7 @@
       <c r="O111" s="15"/>
       <c r="P111" s="15"/>
     </row>
-    <row r="112" spans="1:16" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="112" spans="1:16" s="3" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A112" s="26">
         <v>34</v>
       </c>
@@ -6754,7 +6810,7 @@
         <v>3</v>
       </c>
       <c r="J112" s="15" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="K112" s="18"/>
       <c r="L112" s="15" t="s">
@@ -6765,7 +6821,7 @@
       <c r="O112" s="15"/>
       <c r="P112" s="15"/>
     </row>
-    <row r="113" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1">
+    <row r="113" spans="1:16" s="4" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A113" s="26">
         <v>39</v>
       </c>
@@ -6801,7 +6857,7 @@
       <c r="O113" s="15"/>
       <c r="P113" s="15"/>
     </row>
-    <row r="114" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1">
+    <row r="114" spans="1:16" s="4" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A114" s="26">
         <v>42</v>
       </c>
@@ -6837,7 +6893,7 @@
       <c r="O114" s="15"/>
       <c r="P114" s="15"/>
     </row>
-    <row r="115" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1">
+    <row r="115" spans="1:16" s="4" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A115" s="26">
         <v>43</v>
       </c>
@@ -6873,7 +6929,7 @@
       <c r="O115" s="15"/>
       <c r="P115" s="15"/>
     </row>
-    <row r="116" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1">
+    <row r="116" spans="1:16" s="4" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A116" s="26">
         <v>64</v>
       </c>
@@ -6938,7 +6994,7 @@
       <c r="J117" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="K117" s="15"/>
+      <c r="K117" s="18"/>
       <c r="L117" s="15" t="s">
         <v>218</v>
       </c>
@@ -7019,7 +7075,7 @@
       <c r="O119" s="51"/>
       <c r="P119" s="50"/>
     </row>
-    <row r="120" spans="1:16" s="52" customFormat="1" ht="30" customHeight="1">
+    <row r="120" spans="1:16" s="52" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A120" s="26">
         <v>77</v>
       </c>
@@ -7055,7 +7111,7 @@
       <c r="O120" s="15"/>
       <c r="P120" s="15"/>
     </row>
-    <row r="121" spans="1:16" s="53" customFormat="1" ht="28.8">
+    <row r="121" spans="1:16" s="53" customFormat="1" ht="28.8" hidden="1">
       <c r="A121" s="26">
         <v>80</v>
       </c>
@@ -7091,7 +7147,7 @@
       <c r="O121" s="15"/>
       <c r="P121" s="15"/>
     </row>
-    <row r="122" spans="1:16" s="49" customFormat="1" ht="30" customHeight="1">
+    <row r="122" spans="1:16" s="49" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A122" s="26">
         <v>82</v>
       </c>
@@ -7127,7 +7183,7 @@
       <c r="O122" s="15"/>
       <c r="P122" s="15"/>
     </row>
-    <row r="123" spans="1:16" s="53" customFormat="1" ht="30" customHeight="1">
+    <row r="123" spans="1:16" s="53" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A123" s="26">
         <v>85</v>
       </c>
@@ -7167,7 +7223,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="53" customFormat="1" ht="14.4">
+    <row r="124" spans="1:16" s="53" customFormat="1" ht="28.8" hidden="1">
       <c r="A124" s="26">
         <v>86</v>
       </c>
@@ -7193,8 +7249,12 @@
       <c r="I124" s="15">
         <v>3</v>
       </c>
-      <c r="J124" s="15"/>
-      <c r="K124" s="18"/>
+      <c r="J124" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="K124" s="18" t="s">
+        <v>301</v>
+      </c>
       <c r="L124" s="15" t="s">
         <v>193</v>
       </c>
@@ -7203,7 +7263,7 @@
       <c r="O124" s="15"/>
       <c r="P124" s="15"/>
     </row>
-    <row r="125" spans="1:16" s="53" customFormat="1" ht="30" customHeight="1">
+    <row r="125" spans="1:16" s="53" customFormat="1" ht="30" hidden="1" customHeight="1">
       <c r="A125" s="32">
         <v>114</v>
       </c>
@@ -7261,7 +7321,9 @@
         <v>43136</v>
       </c>
       <c r="I126" s="15"/>
-      <c r="J126" s="15"/>
+      <c r="J126" s="15" t="s">
+        <v>299</v>
+      </c>
       <c r="K126" s="18"/>
       <c r="L126" s="6"/>
       <c r="M126" s="6"/>
@@ -7383,7 +7445,7 @@
     <hyperlink ref="O5" r:id="rId2" display="http://jira.ash.ads.org/browse/ASCS-41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="8" scale="48" orientation="landscape" r:id="rId3"/>
   <tableParts count="1">
     <tablePart r:id="rId4"/>
   </tableParts>

</xml_diff>